<commit_message>
minor update to scheme metadata
</commit_message>
<xml_diff>
--- a/xlsx/skosplay-hips.xlsx
+++ b/xlsx/skosplay-hips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\CODATA\hip-data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471BEEEC-AE2E-4BDA-B64F-E1FA6954F8A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987CBA46-D535-409A-96D4-B4FAFBF15FA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="3465" windowWidth="33105" windowHeight="14100" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
+    <workbookView xWindow="2700" yWindow="3390" windowWidth="33105" windowHeight="14100" activeTab="1" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
   </bookViews>
   <sheets>
     <sheet name="HIPs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -370,6 +370,15 @@
   </si>
   <si>
     <t>https://codata.org/def/hip</t>
+  </si>
+  <si>
+    <t>skos</t>
+  </si>
+  <si>
+    <t>Hazard Information Profiles - provenance</t>
+  </si>
+  <si>
+    <t>Provenance of Descriptions of named hazards, prepared by the ISC/UNDRR Hazard Definitions working group</t>
   </si>
 </sst>
 </file>
@@ -855,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B52F493-8E0A-4796-9035-137B9A6E4DC8}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -957,6 +966,9 @@
     <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1080,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81718AE5-11FE-4358-A679-B2636D311A94}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4"/>
@@ -1216,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4"/>

</xml_diff>

<commit_message>
Synced with official HIP supplement published October 2021
</commit_message>
<xml_diff>
--- a/xlsx/skosplay-hips.xlsx
+++ b/xlsx/skosplay-hips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\CODATA\hip-data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD8908A-245C-4661-8431-A66DF8C5BBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B8744A-2998-4B27-8465-B2C507B1080C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41835" yWindow="3660" windowWidth="32595" windowHeight="15045" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
+    <workbookView xWindow="1230" yWindow="-120" windowWidth="37290" windowHeight="21840" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
   </bookViews>
   <sheets>
     <sheet name="HIPs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>http://www.w3.org/2000/01/rdf-schema#</t>
-  </si>
-  <si>
-    <t>skos:altLabel</t>
   </si>
   <si>
     <r>
@@ -137,49 +134,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>convention-treaty</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>hipo:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
       <t>drivers-outcomes-risk-management</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>hipo:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>references</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>hipo:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>coordinator</t>
     </r>
   </si>
   <si>
@@ -303,49 +258,7 @@
     </r>
   </si>
   <si>
-    <t>World Health Organization (2019). Preventing disease through healthy environments: Exposure to arsenic: A major public health concern. Available at apps.who.int/iris/bitstream/handle/10665/329482/WHO-CED-PHE-EPE-19.4.1-eng.pdf?ua=1. Accessed 21 November 2019.</t>
-  </si>
-  <si>
-    <t>ARSENIC</t>
-  </si>
-  <si>
-    <t>Arsenic is widely distributed throughout the Earth’s crust, generally as arsenic sulphide or as metal arsenates and arsenides. Human exposure to arsenic compounds represents a major public health concern as it has been associated with a range of acute and long-term adverse health effects and diseases (World Health Organization 2019).</t>
-  </si>
-  <si>
-    <t>Arsenic (symbol As, atomic number 33) can be released into the atmosphere and water in the following ways: 
-•	natural activities, such as volcanic activity, dissolution or desorption of minerals (particularly into groundwater), exudates from vegetation and wind-blown dusts; 
-•	human activities, such as metal smelting, combustion of fossil fuels (especially coal), mining, timber treatment with preservatives, and, historically, agricultural pesticide production and use; 
-•	remobilization of historic sources, such as mine drainage water; and 
-•	mobilization into drinking-water from geological deposits by drilling of tube wells (World Health Organization 2019).
-In water, arsenic occurs in one of two main forms: arsenite As(III) under reducing conditions and arsenate As(V) if the water is oxygenated. It can be released to the atmosphere, primarily as the trioxide, mainly by high-temperature processes or through volatilization from aerated soils. In the atmosphere, it is mainly adsorbed on particles, which are dispersed by winds and deposited on land and water (World Health Organization 2019).
-Soluble inorganic arsenic is highly acutely toxic. Intake of inorganic arsenic over a long period can lead to chronic arsenic poisoning (arsenicosis). Effects, which can take years to develop depending on the level of exposure, include skin lesions, peripheral neuropathy, gastrointestinal symptoms, diabetes, cardiovascular disease, developmental toxicity, and cancer of the skin and internal organs (IARC . Organic arsenic compounds, which are abundant in seafood, are less harmful to health and are rapidly eliminated by the body.
-Human exposure to arsenic and arsenic compounds can occur through environmental or occupational routes. Human exposure to elevated levels of inorganic arsenic occurs mainly through the consumption of groundwater containing naturally high levels of inorganic arsenic, food prepared with this water, and food crops irrigated with high-arsenic water sources. Public health actions need to be continued to reduce human exposure to arsenic, particularly in areas with naturally high levels in groundwater (World Health Organization 2019).</t>
-  </si>
-  <si>
-    <t>International Health Regulations
-International Labour Organization C042 - Workmen's Compensation (Occupational Diseases) Convention (Revised), 1934 (No. 42) Available at www.ilo.org/dyn/normlex/en/f?p=NORMLEXPUB:12100:0::NO::P12100_ILO_CODE:C042. Accessed on 21 November 2019.</t>
-  </si>
-  <si>
     <t>https://www.who.int/</t>
-  </si>
-  <si>
-    <t>WHO (2019) reports that arsenic is hazardous in the following ways:
-•	Drinking-water - Drinking-water poses the greatest threat to public health from arsenic (World Health Organization 2019).  
-•	Industrial processes - Most arsenic in industrial processes is used to produce antifungal wood preservatives, which can lead to soil contamination. Other current or historical uses include in the pharmaceutical and glass industries, in the manufacture of alloys, sheep dips, leather preservatives, arsenic-containing pigments, antifouling paints and poison baits and, to a diminishing extent, in the production of agrochemicals (especially for use in orchards and vineyards). Arsenic compounds are also employed in limited amounts in the microelectronics and optical industries. High arsenic levels in air can be found in the working environment as well as the general environment around non-ferrous metal smelters, where arsenic trioxide may be formed, and some coal-fired power plants (especially those using low-grade brown coal) (World Health Organization 2019).
-•	Food - In areas where arsenic is not naturally present at high levels, food usually contributes most to the daily intake of arsenic. Fish, shellfish, meat, poultry, dairy products and cereals are the main sources of dietary intake. However, the arsenic in fish and shellfish is usually in the form of organic compounds (e.g. arsenobetaine) that are of low toxicity. In areas where arsenic is naturally present at high levels, food (e.g. rice) prepared with high arsenic-containing water and food crops irrigated with contaminated water also contribute to total daily intake (World Health Organization 2019).
-•	Smoking - Exposure of smokers to arsenic arises from the natural inorganic arsenic content of tobacco. Exposures were higher in the past when tobacco plants were treated with lead arsenate insecticide (World Health Organization 2019).
-Long-term actions are required to reduce exposure to arsenic from mining, metal smelting and refining, combustion of low-grade coal, pesticide use and timber treatment. In particular, action is needed to reduce the intake of arsenic from drinking-water and food in areas with naturally high levels in the groundwater (World Health Organization 2019).
-The WHO factsheet on Preventing disease through healthy environments - exposure to arsenic: a major public health concern (World Health Organization 2019) includes the following risk mitigation recommendations: 
-•	Make available drinking-water with arsenic concentrations below the WHO provisional drinking-water guideline value of 10 μg/L in areas where the level is higher. Possible measures include: 
-o	testing water for arsenic levels and informing users of the results; 
-o	installing arsenic removal systems, either centralized or domestic, and ensuring appropriate disposal of the removed arsenic; 
-o	substituting high-arsenic sources, such as groundwater, with low-arsenic, microbiologically safe sources such as rainwater and treated surface water. Low-arsenic water can be used for drinking, cooking and irrigation purposes, whereas high-arsenic water can be used for other purposes such as bathing and washing clothes; 
-o	discriminating between high-arsenic and low-arsenic sources by testing water for arsenic levels and painting tube wells or hand pumps different colours (e.g. red and green); and 
-o	blending low-arsenic water with higher-arsenic water to achieve an acceptable arsenic concentration level. 
-•	Reduce occupational exposure to arsenic and its compounds. 
-•	Make both the general public and the health sector aware of the harmful effects of high arsenic intake and the sources of exposure (including use of high-arsenic water for crops irrigation or food preparation) and how to avoid these sources. 
-•	Monitor high-risk populations for early signs of arsenic poisoning, usually skin problems. It should be noted that total urinary arsenic does not differentiate between inorganic arsenic, which is toxic, and organic arsenic, some of which is not. Where possible, arsenic speciation should be attempted in order to differentiate these two forms (and their metabolites). 
-•	The WHO/UNICEF Joint Monitoring Programme for Water Supply, Sanitation and Hygiene monitors progress towards global targets on drinking-water. Under the new 2030 Agenda for Sustainable Development, the indicator of “safely managed drinking water services” calls for tracking the population accessing drinking-water that is free of faecal contamination and priority chemical contaminants, including arsenic.</t>
   </si>
   <si>
     <t>In 2002, WHO (2019) reported that  it was estimated that at least 140 million people in 50 countries have been drinking water containing arsenic at levels above the WHO provisional guideline value of 10 μg/L.3 Inorganic arsenic is naturally present at high levels in the groundwater of a number of countries, such as Argentina, Chile, China, India (West Bengal), Mexico, the United States of America, and particularly Bangladesh, where it was estimated that in 2012 approximately 19 million people were exposed to drinking-water concentrations above the national standard of 50 μg/L and 39 million people were drinking water with levels of arsenic above 10 μg/L.4 In 2010, 21.4% of all deaths in a highly affected area of Bangladesh were attributed to arsenic levels of above 10 μg/L in drinking-water,5 while another analysis published in 2012 for all districts indicated an annual total of nearly 43 000 deaths (about 5.6% of all deaths) attributable to chronic arsenic exposure (World Health Organization 2019).
@@ -355,14 +268,6 @@
 •	Air - A safe level of arsenic in air cannot be established</t>
   </si>
   <si>
-    <t>World Health Organization (2019). Preventing disease through healthy environments: Exposure to arsenic: A major public health concern. Available at apps.who.int/iris/bitstream/handle/10665/329482/WHO-CED-PHE-EPE-19.4.1-eng.pdf?ua=1. Accessed on 21 November 2019.
-•	International Labour Organization (1934). C042 - Workmen's Compensation (Occupational Diseases) Convention (Revised), 1934 (No. 42). Available at www.ilo.org/dyn/normlex/en/f?p=NORMLEXPUB:12100:0::NO::P12100_ILO_CODE:C042. Accessed on 21 November 2019.
-•	International Agency for Research on Cancer (IARC) Arsenic and Arsenic Compounds  : https://monographs.iarc.fr/wp-content/uploads/2018/06/mono100C-6.pdf  Accessed on 3 September 2020</t>
-  </si>
-  <si>
-    <t>hip:arsenic</t>
-  </si>
-  <si>
     <t>hipo:HIP</t>
   </si>
   <si>
@@ -381,47 +286,348 @@
     <t>Provenance of Descriptions of named hazards, prepared by the ISC/UNDRR Hazard Definitions working group</t>
   </si>
   <si>
-    <t>PANDEMIC INFLUENZA</t>
-  </si>
-  <si>
-    <t>An influenza pandemic is a global epidemic caused by a new influenza virus to which there is little or no pre-existing immunity in the human population (World Health Organization 2019).</t>
-  </si>
-  <si>
-    <t>World Health Organization (2019). Pandemic Influenza. Available at http://www.euro.who.int/en/health-topics/communicable-diseases/influenza/pandemic-influenza. Accessed on 19 November 2019.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The constant evolving nature of influenza virus makes influenza among the top few infectious hazards with significant impact. There will be another influenza pandemic. A pandemic occurs when an influenza virus emerges to which there is little or no immunity in the global human population and which can transmit efficiently among people. The pandemic virus can be a virus strain jumping directly from animals or reassorted from animal viruses with or without human seasonal viruses.
-Three influenza pandemics occurred at intervals of several decades during the 20th century, the most severe of which was the so-called ‘Spanish Flu’ (caused by an A(H1N1) virus), estimated to have caused 20–50 million deaths in 1918–19. Milder pandemics occurred subsequently in 1957–58 (the ‘Asian Flu’ caused by an A(H2N2) virus) and in 1968 (the ‘Hong Kong Flu’ caused by an A(H3N2) virus), which were estimated to have caused 1–4 million deaths each. The most recent pandemic was caused by the A(H1N1) virus in 2009.
-The current status of knowledge and technology means that prediction of the next influenza pandemic – when, where, which virus strain, how severe – is impossible. Consequently, pandemic vaccines cannot be developed before the pandemic virus emerges. Innovative research (e.g. at www.who.int/influenza/resources/research/en/) is key to inform and advance pandemic influenza preparedness. Meanwhile, global influenza surveillance, through the WHO Global Influenza Surveillance and Response System (GISRS), timely sharing or viruses and associated information, and national capacity building via seasonal influenza programs are critical to mitigate the impact of inevitable next pandemic.
-</t>
-  </si>
-  <si>
-    <t>The most recent pandemic occurred in 2009 and was caused by an influenza A (H1N1) virus. It is estimated to have caused between 100,000 and 400,000 deaths globally in the first year alone. Children and young adults were disproportionately affected in comparison to seasonal influenza, which causes severe disease mainly in the elderly, persons with chronic conditions and pregnant women (World Health Organization Europe 2019).</t>
-  </si>
-  <si>
-    <t>• International Health Regulations (2005). (World Health Organization 2016).</t>
-  </si>
-  <si>
-    <t>•  Influenza pandemics, whether mild, moderate or severe, affect a large proportion of the population, which puts significant strains on health and other essential services and may result in significant economic losses (World Health Organization Europe 2019).
-• Timely detection, characterization and sharing of the pandemic virus impacts directly the outcome of all downstream response. The WHO Global Influenza Surveillance and Response System (GISRS) is the foundation of such operation. 
-• In an influenza pandemic, the virus is likely to spread rapidly. Rapid development, production and deployment of vaccines is critical to limit the potential impact on populations and essential services (World Health Organization 2019).
-• Access to the appropriate vaccine in the early phases of a pandemic is greatly influenced by global production capacity and the lead-time required to produce influenza vaccines (World Health Organization 2019).
-• As an influenza pandemic may last months or even years, it may require a sustained response in the health sector but also in other sectors providing essential services, such as energy and food production (World Health Organization 2019).</t>
-  </si>
-  <si>
-    <t>•	World Health Organization (2016). International Health Regulations (2005), 3rd ed. Available at www.who.int/ihr/publications/9789241580496/en/. Accessed on 19 November 2019.
-•	World Health Organization (2017). How can I avoid getting the flu? Available at: www.who.int/features/qa/seasonal-influenza/en/. Accessed on 19 November 2019.
-•	World Health Organization (2019). Pandemic Influenza Preparedness. Available at www.who.int/influenza/preparedness/en/. Accessed on 19 November 2019.
-•	World Health Organization (2019). Pandemic Influenza. Available at www.euro.who.int/en/health-topics/communicable-diseases/influenza/pandemic-influenza. Accessed on 19 November 2019.</t>
-  </si>
-  <si>
-    <t>pan flu</t>
-  </si>
-  <si>
-    <t>hip:pandemic-influenza</t>
-  </si>
-  <si>
-    <t>2020-03-01</t>
+    <t>hip:CH0003</t>
+  </si>
+  <si>
+    <t>Arsenic</t>
+  </si>
+  <si>
+    <t>Arsenic is a toxic heavy metal widely distributed throughout the Earth’s crust, generally as arsenic sulphide or as metal arsenates and arsenides. Human exposure to arsenic compounds represents a major public health concern as it has been associated with a range of acute and long-term adverse health effects and diseases (WHO, 2019).</t>
+  </si>
+  <si>
+    <t>WHO, 2019. Preventing Disease through Healthy Environments – Exposure to arsenic: A major public health concern. World Health Organization (WHO). apps.who.int/iris/bitstream/handle/10665/329482/WHO-CED-PHE-EPE-19.4.1-eng.pdf?ua=1 Accessed 21 November 2019.</t>
+  </si>
+  <si>
+    <t>International Labour Organization C042 - Workmen’s Compensation (Occupational Diseases) Convention (Revised), 1934 (ILO, 1934).</t>
+  </si>
+  <si>
+    <t>Drinking-water poses the greatest threat to public health from arsenic (WHO, 2019).
+Most arsenic in industrial processes is used to produce antifungal wood preservatives, which can lead to soil contamination. Other current or historical uses occur within the pharmaceutical and glass industries, in the manufacture of alloys, sheep dips, leather preservatives, arsenic-containing pigments, antifouling paints and poison baits and, to a diminishing extent, in the production of agrochemicals (especially for use in orchards and vineyards). Arsenic compounds are also employed in limited amounts in the microelectronics and optical industries. High arsenic levels in air can be found in the working environment as well as the general environment around non-ferrous metal smelters, where arsenic trioxide may be formed, and some coal-fired power plants (especially those using low-grade brown coal) (WHO, 2019).
+In areas where arsenic is not naturally present at high levels, food usually contributes most to the daily intake of arsenic. Fish, shellfish, meat, poultry, dairy products and cereals are the main sources of dietary intake. However, the arsenic in fish and shellfish is usually in the form of organic compounds (e.g., arsenobetaine) that are of low toxicity. In  areas where arsenic is naturally present at high levels, food (e.g., rice) prepared with high arsenic-containing water and food crops irrigated with contaminated water also contribute to total daily intake (WHO, 2019).
+Exposure of smokers to arsenic arises from the natural inorganic arsenic content of tobacco. Exposures were higher in the past when tobacco plants were treated with lead arsenate insecticide (WHO, 2019).
+Long-term actions are required to reduce exposure to arsenic from mining, metal smelting and refining, combustion of low-grade coal, pesticide use and timber treatment. In particular, action is needed to reduce the intake of arsenic from drinkingwater and food in areas with naturally high levels in the groundwater (WHO, 2019).
+The WHO factsheet on preventing disease through healthy environments (WHO, 2019) includes the following risk mitigation recommendations:
+• Make available drinking-water with arsenic concentrations below the WHO provisional drinking-water guideline value of 10 μg/l in areas where the level is higher. Possible measures include:
+-- Testing water for arsenic levels and informing users of the results.
+-- Installing arsenic removal systems, either centralised or domestic, and ensuring appropriate disposal of the removed arsenic.
+-- Substituting high-arsenic sources, such as groundwater, with low-arsenic, microbiologically safe sources such as rainwater and treated surface water. Low-arsenic water can be used for drinking, cooking and irrigation purposes, whereas higharsenic
+water can be used for other purposes such as bathing and washing clothes.
+-- Discriminating between high-arsenic and low-arsenic sources by testing water for arsenic levels and painting tube wells or hand pumps different colours (e.g., red and green).
+-- Blending low-arsenic water with higher-arsenic water to achieve an acceptable arsenic concentration level.
+• Reduce occupational exposure to arsenic and its compounds.
+• Make both the general public and the health sector aware of the harmful effects of high arsenic intake and the sources of exposure (including use of high-arsenic water for crop irrigation or food preparation) and how to avoid these sources.
+• Monitor high-risk populations for early signs of arsenic poisoning, usually skin problems. It should be noted that total urinary arsenic does not differentiate between inorganic arsenic, which is toxic, and organic arsenic, some of which is not. Where possible, arsenic speciation should be attempted in order to differentiate these two forms (and their metabolites).
+• The WHO/UNICEF Joint Monitoring Programme for Water Supply, Sanitation and Hygiene monitors progress towards global targets on drinking-water. In addition, under the new 2030 Agenda for Sustainable Development, the indicator of ‘safely managed drinking water services’ calls for tracking the population accessing drinking-water that is free of faecal contamination and priority chemical contaminants, including arsenic (UN Water, no date; Council of Europe, 2021).</t>
+  </si>
+  <si>
+    <r>
+      <t>dcterms:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>references</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(separator="|")</t>
+    </r>
+  </si>
+  <si>
+    <t>Council of Europe, 2021. UN Agenda 2030. www.coe.int/en/web/programmes/un-2030-agenda Accessed 7 May 2021.
+|IARC, 2018. Arsenic and Arsenic Compounds. International Agency for Research on Cancer (IARC) https://monographs.iarc.fr/wp-content/uploads/2018/06/mono100C-6.pdf Accessed 3 September 2020.
+|ILO, 1934. C042 - Workmen’s Compensation (Occupational Diseases) Convention (Revised), 1934 (No. 42). International Labour Organization (ILO). www.ilo.org/dyn/normlex/en/f?p=NORMLEXPUB:12100:0::NO::P12100_ILO_CODE:C042 Accessed 21November 2019.
+|UN Water, no date. WHO/UNICEF Joint Monitoring Programme for Water Supply – Sanitation and Hygiene (JMP). www.unwater.org/publication_categories/whounicef-joint-monitoring-programme-for-water-supply-sanitation-hygiene-jmp Accessed 7 May 2021.
+|WHO, 2019. Preventing Disease through Healthy Environments – Exposure to arsenic: A major public health concern. World Health Organization (WHO). apps.who.int/iris/bitstream/handle/10665/329482/WHO-CED-PHE-EPE-19.4.1-eng.pdf?ua=1 Accessed 21 November 2019.</t>
+  </si>
+  <si>
+    <t>Arsenic (chemical symbol As, atomic number 33) can be released into the atmosphere and water in the following ways: natural activities, such as volcanic activity, dissolution or desorption of minerals (particularly into groundwater), exudates from vegetation and wind-blown dusts; human activities, such as metal smelting, combustion of fossil fuels (especially coal), mining, timber treatment with preservatives and, historically, agricultural pesticide production and use; remobilisation of historic sources, such as mine drainage water; and mobilisation into drinking-water from geological deposits by drilling of tube wells (WHO, 2019).
+In water, arsenic occurs in one of two main forms: arsenite As(III) under reducing conditions and arsenate As(V) if the water is oxygenated. It can be released to the atmosphere, primarily as the trioxide, mainly by high-temperature processes or through volatilisation from aerated soils. In the atmosphere, it is mainly adsorbed onto particles, which are dispersed by winds and deposited on land and water (WHO, 2019).
+Soluble inorganic arsenic is highly acutely toxic. Intake of inorganic arsenic over a long period can lead to chronic arsenic poisoning (arsenicosis). Effects, which can take years to develop depending on the level of exposure, include skin lesions, peripheral neuropathy, gastrointestinal symptoms, diabetes, cardiovascular disease, developmental toxicity, and cancer of the skin and internal organs (IARC, 2018). Organic arsenic compounds, which are abundant in seafood, are less harmful to health and are rapidly eliminated by the body.
+Human exposure to arsenic and arsenic compounds can occur through environmental or occupational routes. Human exposure to elevated levels of inorganic arsenic occurs mainly through the intake of groundwater containing naturally high levels of inorganic arsenic, food prepared with this water, and food crops irrigated with high-arsenic water sources. Public health actions need to be continued to reduce human exposure to arsenic, particularly in areas with naturally high levels in groundwater (WHO, 2019).</t>
+  </si>
+  <si>
+    <t>hip:BI0043</t>
+  </si>
+  <si>
+    <t>Pandemic Influenza (Human)</t>
+  </si>
+  <si>
+    <t>An influenza pandemic is the worldwide spread of a new influenza virus to which there is little or no pre-existing immunity in the human population (WHO, 2021).</t>
+  </si>
+  <si>
+    <t>WHO, 2021. World Health Organization (WHO). www.who.int/csr/disease/swineflu/frequently_asked_questions/pandemic/en Accessed June 2021.</t>
+  </si>
+  <si>
+    <t>Pan flu</t>
+  </si>
+  <si>
+    <t>2021-11-05</t>
+  </si>
+  <si>
+    <t>The constantly evolving nature of the influenza virus makes influenza among the top few infectious hazards with significant impact. A pandemic occurs when an influenza virus emerges to which there is little or no immunity in the global human population and which can transmit efficiently among people. The pandemic virus can be a virus strain jumping directly from animals or reassorted from animal viruses with or without human seasonal viruses.
+Three influenza pandemics occurred at intervals of several decades during the 20th century, the most severe of which was the so-called ‘Spanish Flu’ (caused by an A(H1N1) virus), estimated to have caused 20–50 million deaths in 1918–2019. Milder pandemics occurred followed in 1957–1958 (‘Asian Flu’) caused by an A(H2N2) virus) and in 1968 (the ‘Hong Kong Flu’ caused by an A(H3N2) virus), which were estimated to have caused 1–4 million deaths each.
+The current status of knowledge and technology means that predicting the next influenza pandemic – when, where, which virus strain, and how severe it will be – is impossible. Consequently, pandemic vaccines cannot be developed before the pandemic virus emerges. The World Health Organization (WHO) public health research agenda for influenza as an innovative research mechanism is key to inform and advance pandemic influenza preparedness (WHO, 2017a).
+Meanwhile global influenza surveillance, through the WHO Global Influenza Surveillance and Response System (GISRS), assists with timely sharing of virus data and associated information, and national capacity building via seasonal influenza programs that are critical to mitigate the impact of the inevitable next pandemic (WHO, 2017b).</t>
+  </si>
+  <si>
+    <t>The 2009 pandemic was caused by an influenza A (H1N1) virus. It is estimated to have caused between 100,000 and 400,000 deaths globally in the first year alone. Children and young adults were disproportionately affected in comparison to seasonal influenza, which causes severe disease mainly in the elderly, persons with chronic conditions and  pregnant women (WHO, 2019a).</t>
+  </si>
+  <si>
+    <t>International Health Regulations (2005), 3rd ed. (WHO, 2016).</t>
+  </si>
+  <si>
+    <t>Influenza pandemics, whether mild, moderate or severe, affect a large proportion of the global population, which puts significant strains on health and other essential services and may result in significant economic losses (WHO, 2019a).
+Timely detection, characterisation and sharing of information about the pandemic virus directly affects the outcome of all downstream responses. The WHO GISRS is the foundation of such an operation. In an influenza pandemic, the virus is likely to spread rapidly. Rapid development, production and deployment of vaccines is critical to limit the potential impact on populations and essential services (WHO, 2019a).
+Access to the appropriate vaccine in the early phases of a pandemic is greatly influenced by global production capacity and the lead-time required to produce influenza vaccines (WHO, 2019a).
+As an influenza pandemic may last months or even years, it may require a sustained response in the health sector but also in other sectors providing essential services, such as energy and food production (WHO, 2019b).</t>
+  </si>
+  <si>
+    <t>WHO, 2016. International Health Regulations (2005), 3rd ed. World Health Organization (WHO). www.who.int/ihr/publications/
+9789241580496/en Accessed 26 September 2020.
+WHO, 2017a. WHO Public Health Research Agenda for Influenza. World Health Organization (WHO). www.who.int/influenza/
+resources/research/publication_research_agenda_2017/en Accessed 8 November 2020.
+WHO, 2017b. How can I avoid getting the flu? World Health Organization (WHO). www.who.int/features/qa/seasonal-influenza/en Accessed 19 November 2019.
+|WHO, 2019a. Pandemic Influenza. World Health Organization (WHO) Regional Office for Europe. www.euro.who.int/en/healthtopics/communicable-diseases/influenza/pandemic-influenza Accessed 19 November 2019.
+|WHO, 2019b. Pandemic Influenza Preparedness. World Health Organization (WHO). www.who.int/influenza/preparedness/en Accessed 19 November 2019.</t>
+  </si>
+  <si>
+    <t>hip:MH0060</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Wind is air motion relative to the Earth’s surface. Unless otherwise specified, only the horizontal component is considered (WMO, 1992).</t>
+  </si>
+  <si>
+    <t>WMO, 1992. International Meteorological Vocabulary. WMO-No. 182. World Meteorological Organization (WMO). https://library.wmo.int/doc_num.php?explnum_id=4712 Accessed 25 November 2019.</t>
+  </si>
+  <si>
+    <t>Wind velocity is an important consideration in relation to, for example, airborne pollution and the landing of aircraft (WMO, 2018). Surface wind is considered mainly as a two-dimensional vector quantity specified by two numbers representing direction and speed (WMO, 2018).
+The extent to which wind is characterised by rapid fluctuations is referred to as gustiness, and single fluctuations are called gusts (WMO, 2018).</t>
+  </si>
+  <si>
+    <t>An internationally recognised scale for measuring wind is the Beaufort Scale, which is an empirical measure that relates wind speed to observed conditions at sea or on land. Its full name is the Beaufort wind force scale (Royal Meteorological Society, 2018).
+The Beaufort wind force scale has 13 levels including: calm, light air, light breeze, gentle breeze, moderate breeze, fresh breeze, strong breeze, near gale, gale, strong gale, storm, violent storm, and hurricane. Of note, the quoted wind speed is that measured at 10 m above ground, not at the surface (which, at 2 m, may be only 50–70% of these values  (Royal Meteorological Society, 2018).</t>
+  </si>
+  <si>
+    <t>Not identified.</t>
+  </si>
+  <si>
+    <t>Wind is a main or contributing component to a number of hazards such as derecho, tropical cyclone, blizzard, sub-tropical cyclone, subtropical storm, tornado, and tropical storm. Wind is also associated with the dispersal of dust storms, volcanic ash and coastal floods (WMO, 2019).
+Human health can be severely affected by windstorms (Goldman et al., 2014). Effects include direct effects, which occur during the impact phase of a storm, causing death and injury due to the force of the wind. Becoming airborne, being struck by flying debris or falling trees and road traffic accidents are the main dangers. Indirect effects, occurring  during the pre- and postimpact phases of the storm, include falls, lacerations and puncture wounds, and occur when preparing for, or cleaning up after a storm. Power outages are a key issue and can lead to electrocution, fires and burns, and carbon monoxide poisoning from gasoline powered electrical generators. Worsening of chronic illnesses due to lack of access to medical care or medication can also occur. Other health impacts include infections and insect bites.</t>
+  </si>
+  <si>
+    <t>Goldman, A., B. Eggen, B. Golding and V. Murray, 2014. The health impacts of windstorms: a systematic literature review. Public
+Health, 128:3-28.
+| Royal Meteorological Society, 2018. The Beaufort Scale. www.rmets.org/resource/beaufort-scale Accessed 9 November 2020.
+| WMO, 2018. Guide to Instruments and Methods of Observation. Volume I – Measurement of Meteorological Variables. WMONo. 8. World Meteorological Association (WMO). https://library.wmo.int/?lvl=notice_display&amp;id=12407#.YJ0upiuSk2w Accessed 9 November 2020.
+| WMO, 2019. Event Types of Hazards and Extreme Events. World Meteorological Association (WMO). www.wmo.int/pages/prog/wcp/wcdmp/meeting/documents/Catalogue_Hazards_Extreme_Events_WMO_091117.pdf Accessed 9 November 2020.</t>
+  </si>
+  <si>
+    <t>https://www.wmo.int</t>
+  </si>
+  <si>
+    <t>hip:CH0020</t>
+  </si>
+  <si>
+    <t>Asbestos</t>
+  </si>
+  <si>
+    <t>Asbestos is the term for a group of naturally occurring minerals widely used historically in building materials and other products (WHO, no date). All types of asbestos cause lung cancer, mesothelioma, cancer of the larynx and ovary, and asbestosis (fibrosis of the lungs) (WHO, no date).</t>
+  </si>
+  <si>
+    <t>WHO, no date. International Programme on Chemical Safety: Asbestos. World Health Organization (WHO). www.who.int/ipcs/assessment/public_health/asbestos/en Accessed 18 November 2019.</t>
+  </si>
+  <si>
+    <t>Asbestos has current or historical commercial use due to its extraordinary tensile strength, poor heat conduction, and relative resistance to chemical attack. For these reasons, asbestos is used for insulation in buildings and as an ingredient in a number of products, such as roofing shingles, water supply lines, and fire blankets, as well as clutches and brake linings, gaskets, and pads for automobiles (WHO, no date).
+The main forms of asbestos are chrysotile (white asbestos) and crocidolite (blue asbestos). Other forms include amosite, anthophylite, tremolite and actinolite (WHO, no date).
+All forms of asbestos are carcinogenic to humans. Exposure to asbestos, including chrysotile, causes cancer of the lung, larynx, and ovaries, and also mesothelioma (a cancer of the pleural and peritoneal linings). Asbestos exposure is also responsible for other diseases such as asbestosis (fibrosis of the lungs), and plaques, thickening and effusion in the pleura (WHO, no date).</t>
+  </si>
+  <si>
+    <t>According to the World Health Organization (WHO), globally about 125 million people are currently exposed to asbestos at the workplace. In 2004, asbestos-related lung cancer, mesothelioma and asbestosis from occupational exposure resulted in 107,000 deaths and 1523,000 Disability Adjusted Life Years (DALYs) (WHO, no date). In addition, nearly 400 deaths have been attributed to non-occupational exposure to asbestos. The burden of asbestos-related diseases is still rising, even in countries that banned its use in the early 1990s. Owing to the long latency periods attached to the diseases in question, stopping the use of asbestos now will only result in a decrease in the number of asbestos-related deaths after a number of decades (WHO, 2014).
+The WHO air quality guidelines for Europe estimate likely lifetime exposure for asbestos based on typical environmental concentrations and the associated health risk factors such as mesothelomia and lung cancer (WHO, 2000:38).</t>
+  </si>
+  <si>
+    <r>
+      <t>hipo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>convention-treaty</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(separator="|")</t>
+    </r>
+  </si>
+  <si>
+    <t>Asbestos Convention, 1986 (ILO, 1962).
+|Basel Convention on the Control of Transboundary Movements of Hazardous Wastes and their Disposal (Basel Convention, 1989). At the time of writing, there were 187 parties to the Basel Convention.</t>
+  </si>
+  <si>
+    <t>In many disaster-prone areas, asbestos cement is widely used as a building material and when the material corrodes due to aging or is damaged it releases harmful asbestos fibres. Fires in buildings can release large amounts of dust and fibres from asbestos and fibreglass insulation (WHO, 2018).
+The WHO, in collaboration with the International Labour Organization and other intergovernmental organisations and civil society, works with countries towards elimination of asbestos-related diseases by (WHO, no date):
+• Recognising that the most efficient way to eliminate asbestos-related diseases is to stop the use of all types of asbestos.
+• Providing information about solutions for replacing asbestos with safer substitutes and developing economic and technological mechanisms to stimulate its replacement.
+• Taking measures to prevent exposure to asbestos in place and during asbestos removal (abatement).
+• Improving early diagnosis, treatment, and rehabilitation services for asbestos-related diseases.
+• Establishing registries of people with past and/or current exposures to asbestos and organising medical surveillance of exposed workers.
+• Providing information on the hazards associated with asbestos-containing materials and products, and by raising awareness that waste containing asbestos should be treated as hazardous waste.
+Cost-effective interventions for preventing occupational lung diseases from exposure to asbestos are among the policy options for implementing the Global Action Plan for the Prevention and Control of Noncommunicable Diseases (2013-2020), as endorsed by the Sixty-sixth World Health Assembly in 2013 (WHO, 2013).
+Asbestos is a proven human carcinogen (International Agency for Research on Cancer [IARC] Group 1). No safe level can be proposed for asbestos because a threshold is not known to exist. Exposure should therefore be kept as low as possible (IARC, 1987/1998).</t>
+  </si>
+  <si>
+    <t>Basel Convention, 1989. Basel Convention on the Control of Transboundary Movements of Hazardous Wastes and their Disposal (1989). At the time of writing, there were 187 parties to the Basel Convention. Official website: www.basel.int Accessed 18 November 2019.
+|IARC, 1987. Asbestos (Actinolite, amosite, anthophyllite, chrysotile, crocidolite, tremolite) (Group 1). Summaries &amp; Evaluations Supplement 7:106. Last updated 1998. International Agency for Research on Cancer (IARC). www.inchem.org/documents/iarc/suppl7/asbestos.html Accessed 18 November 2019.
+|ILO, 1962. C162 - Asbestos Convention, 1986 (No. 162). International Labour Organization (ILO). www.ilo.org/dyn/normlex/en/f?p=NORMLEXPUB:12100:0::NO::P12100_ILO_CODE:C162. Accessed 18 November 2019.
+|WHO, no date. International Programme on Chemical Safety: Asbestos. World Health Organization (WHO). www.who.int/ipcs/assessment/public_health/asbestos/en Accessed 18 November 2019.
+|WHO, 2013. Global action plan for the prevention and control of noncommunicable diseases 2013-2020. World Health Organization (WHO). apps.who.int/iris/bitstream/handle/10665/94384/9789241506236_eng.pdf;jsessionid=431E06013F1E86614BB088F7CCA30759?sequence=1 Accessed 18 November 2019.
+|WHO, 2014. Chrysotile asbestos. World Health Organization (WHO). apps.who.int/iris/bitstream/handle/10665/143649/9789241564816_eng.pdf?sequence=1 Accessed 18 November 2019.
+|WHO, 2018. Chemical releases caused by natural hazard events and disasters: Information for public health authorities. World Health Organization (WHO). apps.who.int/iris/bitstream/handle/10665/272390/9789241513395-eng.pdf?ua=1 Accessed 18 November 2019.
+|WHO, 2000. Air Quality Guidelines for Europe, Second Edition. World Health Organization (WHO) Regional Office for Europe. European Series, No. 91. www.euro.who.int/__data/assets/pdf_file/0005/74732/E71922.pdf?ua=1 Accessed 18 November 2019.</t>
+  </si>
+  <si>
+    <r>
+      <t>hipo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>coordinator</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(separator="|")</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.who.int/health-topics/chemical-safety</t>
+  </si>
+  <si>
+    <t>hip:BI0030</t>
+  </si>
+  <si>
+    <t>Hepatitis B (Human)</t>
+  </si>
+  <si>
+    <t>Hepatitis B is a vaccine-preventable disease, that is endemic and epidemic worldwide, and caused by the Hepatitis B virus (HBV). HBV can cause both acute and chronic liver disease. Chronic infection puts people at high risk of death from cirrhosis and liver cancer (WHO, 2020).</t>
+  </si>
+  <si>
+    <t>WHO, 2020. Hepatitis B. World Health Organization (WHO). www.who.int/news-room/fact-sheets/detail/hepatitis-b Accessed 8 November 2020.</t>
+  </si>
+  <si>
+    <t>skos:altLabel(separator="|")</t>
+  </si>
+  <si>
+    <t>Hepatitis B is the most serious type of viral hepatitis. In highly endemic areas, the Hepatitis B virus (HBV), which is highly contagious, is most commonly spread from mother to child at birth (perinatal transmission), or through horizontal transmission (exposure to infected blood), especially from an infected child to an uninfected child during the first five years of life (WHO, 2016a).
+Hepatitis B is also spread by needlestick injury, tattooing, piercing and exposure to infected blood and body fluids, such as saliva and, menstrual, vaginal, and seminal fluids. Sexual transmission of hepatitis B may occur, particularly in unvaccinated men who have sex with men and heterosexual persons with multiple sex partners or contact with sex workers (WHO, 2020).
+The incubation period of the HBV is 75 days on average but can vary from 30 to 180 days. Most people do not experience any symptoms when newly infected. However, some have acute illness with symptoms that last several weeks, including yellowing of the skin and eyes (jaundice), dark urine, extreme fatigue, nausea, vomiting and abdominal pain. A small subset of persons with acute hepatitis can develop acute liver failure, which can lead to death (WHO, 2020).
+In some people, the HBV can also cause a chronic liver infection that can later develop into cirrhosis (a scarring of the liver) or hepatocellular carcinoma (liver cancer). Infection in adulthood leads to chronic hepatitis in less than 5% of cases, whereas infection in infancy and early childhood leads to chronic hepatitis in about 95% of cases (WHO, 2020).
+Laboratory confirmation of hepatitis B diagnosis is essential. A number of blood tests are available to diagnose and monitor people with hepatitis B. They can be used to distinguish acute and chronic infections (WHO, 2020).
+The World Health Organisation (WHO) has published surveillance standards for hepatitis B (WHO, no date).</t>
+  </si>
+  <si>
+    <t>The prevalence of hepatitis B is highest in the WHO Western Pacific Region and the WHO African Region, where 6.2% and 6.1% of the adult population is infected respectively (WHO, 2020).
+In the WHO Eastern Mediterranean Region, the WHO South-East Asia Region and the WHO European Region, an estimated 3.3%, 2.0% and 1.6% of the general population is infected, respectively (WHO, 2020).
+In the WHO Region of the Americas, 0.7% of the population is infected (WHO, 2017).
+The WHO estimates that in 2015, 257 million people were living with chronic hepatitis B infection (defined as hepatitis B surface antigen positive) (WHO, 2019). It is estimated that about 887,000 people die each year due to consequences of hepatitis B (WHO, 2017).
+HBV-HIV coinfection: about 1% of persons living with HBV infection (2.7 million people) are also infected with human immunodeficiency virus (HIV). Conversely, the global prevalence of HBV infection in HIV-infected persons is 7.4% (WHO, 2019).</t>
+  </si>
+  <si>
+    <t>International Health Regulations (2005), 3rd ed. (WHO, 2016b).</t>
+  </si>
+  <si>
+    <t>Hepatitis B is a major global health problem (WHO, 2018). However, there is still limited access to diagnosis and treatment of hepatitis B in many resource-constrained settings. In 2016, 10.5% (27 million) of those infected were aware of their infection. Of those diagnosed, the global treatment coverage is 16.7% (4.5 million). Many people are diagnosed only when they already have advanced liver disease (WHO, 2019, 2020).
+A safe and effective vaccine that offers 98–100% protection against hepatitis B is available and is the mainstay of prevention worldwide (WHO, 2020).
+The WHO recommends that all blood donations be tested for hepatitis B to ensure blood safety and avoid accidental transmission to people who receive blood products (WHO, 2020).
+For World Hepatitis Day 2020, the WHO focused on the theme ‘Hepatitis-Free Future’ to highlight the importance of addressing the prevention of mother-to-child transmission of HBV; to launch new guidance; and to call for increased domestic and international programming and funding to prevent hepatitis B mother-to-child transmission, as well as to expand access to hepatitis prevention, testing and treatment services, with a view to achieving the 2030 elimination targets (WHO, 2020).</t>
+  </si>
+  <si>
+    <t>WHO, no date. Immunizations, Vaccines and Biologicals: WHO-recommended Surveillance Standard of Acute Viral Hepatitis. World Health Organization (WHO). www.who.int/immunization/monitoring_surveillance/burden/vpd/surveillance_type/passive/hepatitis_standards/en Accessed 21 November 2019.
+|WHO, 2016a. Technical considerations and case definitions to improve surveillance for viral hepatitis: technical report. World Health Organization (WHO). https://apps.who.int/iris/handle/10665/204501 Accessed 18 February 2020.
+|WHO, 2016b. International Health Regulations (2005), 3rd ed. World Health Organization (WHO). www.who.int/ihr/publications/9789241580496/en Accessed 26 September 2020.
+|WHO, 2017. Global Hepatitis Report 2017. World Health Organization (WHO). www.who.int/hepatitis/publications/globalhepatitis-report2017/en Accessed 18 February 2020.
+|WHO, 2018. Immunizations, Vaccines and Biologicals: Hepatitis B. World Health Organization (WHO). www.who.int/immunization/diseases/hepatitisB/en Accessed 21 November 2019.
+|WHO, 2019. Progress report on HIV, viral hepatitis and sexually transmitted infections 2019: accountability for the global health sector strategies, 2016–2021. World Health Organization (WHO). www.who.int/hiv/strategy2016-2021/progress-report-2019/en Accessed 18 February 2020.
+|WHO, 2020. Hepatitis B. World Health Organization (WHO). www.who.int/news-room/fact-sheets/detail/hepatitis-b Accessed 8 November 2020.</t>
+  </si>
+  <si>
+    <t>hip:MH0050</t>
+  </si>
+  <si>
+    <t>Avalanche</t>
+  </si>
+  <si>
+    <t>An avalanche is a mass of snow and ice falling suddenly down a mountain slope and often taking with it earth, rocks and rubble of every description (WMO, 1992).</t>
+  </si>
+  <si>
+    <t>WMO, 1992. International Meteorological Vocabulary. WMO-No. 182. World Meteorological Organization (WMO). https://library.wmo.int/doc_num.php?explnum_id=4712 Accessed 4 December 2019.</t>
+  </si>
+  <si>
+    <t>An avalanche is a rapid flow of snow down a hill or mountainside (NSIDC, 2021). Although avalanches can occur on any slope given the right conditions, certain times of the year and certain locations are more dangerous than others. Winter, particularly from December to April in the Northern Hemisphere, is when most avalanches tend to happen (NSIDC, no date).
+There are different types of avalanche (SLF, no date a):
+• Loose snow avalanches start from a single point and form when snow is not well bonded. A loose snow avalanche consisting of dry powder generally requires a slope angle of 40°. In very steep terrain, as individual snow particles become loose, roll downwards and bump into more particles, they form an inverted-V-shaped avalanche. Because loose snow avalanches usually carry less snow and travel more slowly than slab avalanches, they are also less dangerous.
+• Slab avalanches can only form when the snowpack comprises multiple layers of snow. Slab avalanches are characterised by the simultaneous release of a cohesive snow layer (slab). Steeper than around 30°, slab avalanches are usually bigger than a typical skier avalanche (which is on average 50 m wide, 150–200 m long and 50 cm thick) and reach speeds of 50–100 km/h.
+• Gliding avalanches, like slab avalanches, have a distinct, broad fracture line, but differ from other types of avalanches in as much as the entire snowpack is released. The slope must be sufficiently steep, but gliding can occur at a slope angle of just 15°. Gliding avalanches can occur only on a smooth substrata, typically consisting of flattened grass or slabs of rock.
+• Powder avalanches arise mostly from slab avalanches. A powder cloud forms in the presence of a large altitude difference when a sufficient quantity of snow becomes suspended in the air. Powder avalanches can reach speeds of 300 km/h and cause tremendous damage.
+• Wet-snow avalanches are usually triggered naturally, most often by a big rise in temperature. Meltwater or occasionally rainwater penetrating the snowpack weakens the bonds between the snow crystals, thereby destabilising layers in which the water accumulates. Both loose snow avalanches and slab avalanches can consist of wet snow.</t>
+  </si>
+  <si>
+    <t>Not available.</t>
+  </si>
+  <si>
+    <t>Avalanche danger is enhanced in some circumstances, commonly in windy conditions on fresh snow slopes; when there is rapid, significant, warming of the snow to above 0°; and on steeper, shadier slopes (White risk, no date).
+Avalanche protection and control measures include early warning which is key. The European Avalanche Warning Services (EAWS) brings together 29 avalanche warning services from 16 countries (EAWS, 2020).
+By way of controlled explosions, artificial avalanche triggering aims temporarily to safeguard possible starting zones, avalanche paths and deposition zones, and to prevent large avalanches and lengthy closures (SLF, no date b).
+Defensive structures prevent the formation of avalanches. In other circumstances, when an avalanche is released, it can be diverted or intercepted by a dam. Other means of protection against avalanches include physical structures for buildings and snow sheds. In order to stop an avalanche completely, depending on its speed, a dam may need to be more than 20 m high. Many dams have a dual function: they protect against avalanches in winter, and against flooding and debris flows once the snow has melted. Snow sheds are known as avalanche galleries or tunnels, and are the classic structures for protecting transportation routes. Among the typical measures for protecting buildings are wall reinforcement, the erection of a solid structure (Spaltkeil), which is rather like a log splitting wedge, to break the avalanche, and a building design (Ebenhöch) in which the roof seamlessly merges with the terrain or an embankment (SLF, no date c).</t>
+  </si>
+  <si>
+    <t>EAWS, 2020. Our Mission. European Avalanche Warning Services (EAWS). www.avalanches.org Accessed 25 March 2021.
+|NSIDC, no date. All about snow: Snow avalanches. National Snow and Ice Data Center (NSIDC). nsidc.org/cryosphere/snow/science/avalanches.html Accessed 4 December 2019.
+|NSIDC, 2021. Cryosphere Glossary: Avalanche. National Snow and Ice Data Center (NSIDC). https://nsidc.org/cryosphere/glossary/term/avalanche Accessed 25 March 2021.
+|SLF, no date a. Avalanche protection. WSL Institute for Snow Avalanche Research SLF. www.slf.ch/en/avalanches/avalancheprotection.html Accessed on 4 December 2019.
+|SLF, no date b. Artificial Avalanche Triggering. www.slf.ch/en/avalanches/avalanche-protection/artificial-avalanche-triggering.html Accessed 25 March 2021.
+|SLF, no date c. WSL Institute for Snow and Avalanche Research SLF. www.wsl.ch/en/about-wsl/locations/slf-davos.html Accessed 25 March 2021.
+|White Risk, no date. Effect of Weather and Temperature on Avalanche Hazard. https://whiterisk.ch/de/explore#u=05-02-08-05 Accessed 25 March 2021.</t>
+  </si>
+  <si>
+    <t>Acute hepatitis B|Chronic hepatitis B|Hepatitis B related cirrhosis and hepatocellular carcinoma</t>
   </si>
 </sst>
 </file>
@@ -587,18 +793,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -915,20 +1119,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B52F493-8E0A-4796-9035-137B9A6E4DC8}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="15" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <pane xSplit="3" ySplit="13" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="59" style="4" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="30" style="4" customWidth="1"/>
     <col min="6" max="6" width="85" style="4" customWidth="1"/>
@@ -945,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -986,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>12</v>
@@ -997,10 +1201,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1008,10 +1212,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1035,150 +1239,295 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C13" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F13" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="H13" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="M15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="19" t="s">
+      <c r="J13" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="N13" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="22">
+        <v>44505</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="25" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="21" customFormat="1" ht="390" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>48</v>
+        <v>72</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>73</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>51</v>
+        <v>75</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>76</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="L16" s="22">
-        <v>44077</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="27" customFormat="1" ht="390" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="K17" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" s="27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="25"/>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="24"/>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="25"/>
-      <c r="I20" s="24"/>
+    </row>
+    <row r="17" spans="1:13" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F21" s="24"/>
-      <c r="I21" s="24"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F22" s="13"/>
@@ -1189,15 +1538,12 @@
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F26" s="13"/>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K19" r:id="rId1" display="https://www.wmo.int/pages/index_en.html" xr:uid="{897E53C1-C243-456B-BD5F-8D87D9197DD5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1230,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1279,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>12</v>
@@ -1292,10 +1638,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1305,10 +1651,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1318,10 +1664,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1331,7 +1677,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4"/>
@@ -1342,7 +1688,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4"/>
@@ -1380,16 +1726,16 @@
         <v>6</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -1403,22 +1749,22 @@
     </row>
     <row r="17" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hid first 13 rows
Hid first 13 rows
</commit_message>
<xml_diff>
--- a/xlsx/skosplay-hips.xlsx
+++ b/xlsx/skosplay-hips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\CODATA\hip-data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Simon_Gato_1/Documents/GitHub/hip-data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B8744A-2998-4B27-8465-B2C507B1080C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5754F92C-C058-0B48-86D8-F583366903A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="-120" windowWidth="37290" windowHeight="21840" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
   </bookViews>
   <sheets>
     <sheet name="HIPs" sheetId="1" r:id="rId1"/>
@@ -1122,29 +1122,29 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="13" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="13" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" sqref="A1:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="46.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="33.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="30" style="4" customWidth="1"/>
     <col min="6" max="6" width="85" style="4" customWidth="1"/>
-    <col min="7" max="7" width="61.140625" style="4" customWidth="1"/>
-    <col min="8" max="10" width="46.28515625" style="4"/>
-    <col min="11" max="11" width="25.42578125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="61.1640625" style="4" customWidth="1"/>
+    <col min="8" max="10" width="46.33203125" style="4"/>
+    <col min="11" max="11" width="25.5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" style="4" customWidth="1"/>
     <col min="13" max="13" width="22" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="46.28515625" style="4"/>
+    <col min="14" max="16384" width="46.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
@@ -1234,7 +1234,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:14" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1242,10 +1243,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
     </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>5</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="21" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>49</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>44505</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="25" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="25" customFormat="1" ht="380" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>58</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="21" customFormat="1" ht="390" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="21" customFormat="1" ht="335" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>69</v>
       </c>
@@ -1406,7 +1407,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="21" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>79</v>
       </c>
@@ -1444,7 +1445,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="21" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>91</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>101</v>
       </c>
@@ -1523,19 +1524,19 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F24" s="13"/>
     </row>
   </sheetData>
@@ -1555,23 +1556,23 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="64.140625" style="5" customWidth="1"/>
-    <col min="6" max="9" width="21.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="35.7109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="49.28515625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="30.28515625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="18.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="41.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="64.1640625" style="5" customWidth="1"/>
+    <col min="6" max="9" width="21.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="49.33203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="23.83203125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="30.33203125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="21.5" style="5" customWidth="1"/>
+    <col min="15" max="16384" width="9.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1581,7 +1582,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1594,7 +1595,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1607,7 +1608,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1620,7 +1621,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1633,7 +1634,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1646,7 +1647,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1659,7 +1660,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1672,7 +1673,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1683,7 +1684,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1694,31 +1695,31 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1748,7 @@
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
@@ -1767,13 +1768,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D20" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean out metadata sheet
</commit_message>
<xml_diff>
--- a/xlsx/skosplay-hips.xlsx
+++ b/xlsx/skosplay-hips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\CODATA\hip-data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B8744A-2998-4B27-8465-B2C507B1080C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94344590-02EF-45A7-83F5-C018D288CAFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="-120" windowWidth="37290" windowHeight="21840" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
+    <workbookView xWindow="4620" yWindow="4710" windowWidth="17970" windowHeight="16095" activeTab="1" xr2:uid="{C6941A0D-9C17-41CC-B9DE-403EB2C5F0A5}"/>
   </bookViews>
   <sheets>
     <sheet name="HIPs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -138,37 +138,9 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>hipo:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Provenance</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">hip </t>
   </si>
   <si>
-    <r>
-      <t>hip:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>_arsenic</t>
-    </r>
-  </si>
-  <si>
     <t>owl</t>
   </si>
   <si>
@@ -197,40 +169,6 @@
   </si>
   <si>
     <t>hipp</t>
-  </si>
-  <si>
-    <t>hipp:lidia-mayner , hipp:virginia-murray</t>
-  </si>
-  <si>
-    <t>4.0 Reviewed and updates
-3.0 Lidia Mayner reviewed and updated 11 November 2019
-2.0 Lidia Mayer reviewed and updated 18 October 2019
-1.0 Lidia Mayer 6 August 2019, Virginia Murray reviewed 7 August 2019</t>
-  </si>
-  <si>
-    <t>Version: 
-4.0 Reviewed and updates
-3.0 Lidia Mayner reviewed and updated 11 November 2019
-2.0 Lidia Mayer reviewed and updated 18 October 2019
-1.0 Lidia Mayer 6 August 2019, Virginia Murray reviewed 7 August 2019
-Initial Review: 
-Contact Email: Virginia.Murray@phe.gov.uk 
-External reviewers include John Duffus, Mike Schwenk, IUTOX, Daniel Vallero
-FINAL Virginia Murray 3 September 2020</t>
-  </si>
-  <si>
-    <r>
-      <t>hip:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>arsenic</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1121,11 +1059,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B52F493-8E0A-4796-9035-137B9A6E4DC8}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="13" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="13" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1190,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>12</v>
@@ -1201,10 +1139,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1212,10 +1150,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1239,7 +1177,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1268,22 +1206,22 @@
         <v>21</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="N13" s="19" t="s">
         <v>9</v>
@@ -1291,37 +1229,37 @@
     </row>
     <row r="14" spans="1:14" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C14" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>56</v>
-      </c>
       <c r="K14" s="21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L14" s="22">
         <v>44505</v>
@@ -1329,198 +1267,198 @@
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="G15" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="H15" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="I15" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>67</v>
-      </c>
       <c r="J15" s="25" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L15" s="24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="M15" s="25" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="21" customFormat="1" ht="390" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="I16" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="J16" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="K16" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="K16" t="s">
-        <v>78</v>
-      </c>
       <c r="L16" s="24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C17" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="I17" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="J17" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="21" t="s">
+      <c r="K17" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>90</v>
-      </c>
       <c r="L17" s="24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="21" t="s">
+      <c r="H18" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="I18" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="J18" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>100</v>
-      </c>
       <c r="K18" s="21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="K19" s="27" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L19" s="24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1551,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81718AE5-11FE-4358-A679-B2636D311A94}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1625,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>12</v>
@@ -1638,10 +1576,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1651,10 +1589,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1664,10 +1602,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1677,7 +1615,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4"/>
@@ -1688,7 +1626,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4"/>
@@ -1726,16 +1664,16 @@
         <v>6</v>
       </c>
       <c r="C16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -1747,25 +1685,13 @@
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>39</v>
-      </c>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D18" s="14"/>

</xml_diff>